<commit_message>
reduce total expenses to better represent a logical income to expense ratio
</commit_message>
<xml_diff>
--- a/data/sample/sample.xlsx
+++ b/data/sample/sample.xlsx
@@ -201,17 +201,23 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -224,16 +230,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -250,16 +256,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -279,6 +285,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -478,12 +485,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -506,7 +513,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -516,10 +522,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -536,7 +542,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -562,7 +567,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -588,7 +592,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -614,7 +617,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -640,7 +642,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -666,7 +667,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -692,7 +692,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -718,7 +717,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -744,7 +742,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -767,12 +764,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -795,7 +792,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -821,7 +817,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -847,7 +842,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -873,7 +867,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -899,7 +892,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -925,7 +917,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -951,7 +942,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -977,7 +967,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1003,7 +992,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1029,7 +1017,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1077,7 +1064,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1087,10 +1073,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1107,7 +1093,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1133,7 +1118,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1159,7 +1143,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1185,7 +1168,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1211,7 +1193,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1237,7 +1218,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1263,7 +1243,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1289,7 +1268,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1315,7 +1293,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1414,7 +1391,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="4">
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="D3" s="5">
         <v>44927</v>
@@ -1658,7 +1635,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="4">
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="D13" s="5">
         <v>45200</v>
@@ -1902,7 +1879,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="4">
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="D23" t="s" s="2">
         <v>44</v>
@@ -2146,7 +2123,7 @@
         <v>12</v>
       </c>
       <c r="C33" s="4">
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="D33" t="s" s="2">
         <v>54</v>

</xml_diff>

<commit_message>
change category name of secondary income sources to Income
</commit_message>
<xml_diff>
--- a/data/sample/sample.xlsx
+++ b/data/sample/sample.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>Type</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Freelance Project</t>
-  </si>
-  <si>
-    <t>Career</t>
   </si>
   <si>
     <t>Web development</t>
@@ -1447,11 +1444,11 @@
         <v>44986</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" t="s" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1461,7 +1458,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4">
         <v>40</v>
@@ -1470,13 +1467,13 @@
         <v>44986</v>
       </c>
       <c r="E6" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="F6" t="s" s="2">
+      <c r="G6" t="s" s="2">
         <v>24</v>
-      </c>
-      <c r="G6" t="s" s="2">
-        <v>25</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1486,7 +1483,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4">
         <v>200</v>
@@ -1495,11 +1492,11 @@
         <v>45017</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" t="s" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1509,7 +1506,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4">
         <v>150</v>
@@ -1518,13 +1515,13 @@
         <v>45047</v>
       </c>
       <c r="E8" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="F8" t="s" s="2">
+      <c r="G8" t="s" s="2">
         <v>30</v>
-      </c>
-      <c r="G8" t="s" s="2">
-        <v>31</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1534,7 +1531,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="4">
         <v>120</v>
@@ -1543,11 +1540,11 @@
         <v>45078</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1557,7 +1554,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="4">
         <v>60</v>
@@ -1569,10 +1566,10 @@
         <v>16</v>
       </c>
       <c r="F10" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s" s="2">
         <v>35</v>
-      </c>
-      <c r="G10" t="s" s="2">
-        <v>36</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1691,11 +1688,11 @@
         <v>45261</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" t="s" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -1705,22 +1702,22 @@
         <v>11</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4">
         <v>40</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="F16" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="F16" t="s" s="2">
+      <c r="G16" t="s" s="2">
         <v>24</v>
-      </c>
-      <c r="G16" t="s" s="2">
-        <v>25</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1730,20 +1727,20 @@
         <v>7</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="4">
         <v>200</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" t="s" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1753,22 +1750,22 @@
         <v>11</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="4">
         <v>150</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="F18" t="s" s="2">
+      <c r="G18" t="s" s="2">
         <v>30</v>
-      </c>
-      <c r="G18" t="s" s="2">
-        <v>31</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1778,20 +1775,20 @@
         <v>7</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4">
         <v>120</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1801,22 +1798,22 @@
         <v>11</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="4">
         <v>60</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" t="s" s="2">
         <v>16</v>
       </c>
       <c r="F20" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="G20" t="s" s="2">
         <v>35</v>
-      </c>
-      <c r="G20" t="s" s="2">
-        <v>36</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -1832,7 +1829,7 @@
         <v>80</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s" s="2">
         <v>16</v>
@@ -1857,7 +1854,7 @@
         <v>1800</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" t="s" s="2">
         <v>7</v>
@@ -1882,7 +1879,7 @@
         <v>800</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s" s="2">
         <v>13</v>
@@ -1907,7 +1904,7 @@
         <v>75.5</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s" s="2">
         <v>16</v>
@@ -1932,14 +1929,14 @@
         <v>300</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" t="s" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -1949,22 +1946,22 @@
         <v>11</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="4">
         <v>40</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="F26" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="F26" t="s" s="2">
+      <c r="G26" t="s" s="2">
         <v>24</v>
-      </c>
-      <c r="G26" t="s" s="2">
-        <v>25</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1974,20 +1971,20 @@
         <v>7</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="4">
         <v>200</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" t="s" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" t="s" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -1997,22 +1994,22 @@
         <v>11</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="4">
         <v>150</v>
       </c>
       <c r="D28" t="s" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="F28" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="F28" t="s" s="2">
+      <c r="G28" t="s" s="2">
         <v>30</v>
-      </c>
-      <c r="G28" t="s" s="2">
-        <v>31</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -2022,20 +2019,20 @@
         <v>7</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="4">
         <v>120</v>
       </c>
       <c r="D29" t="s" s="2">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -2045,22 +2042,22 @@
         <v>11</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="4">
         <v>60</v>
       </c>
       <c r="D30" t="s" s="2">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30" t="s" s="2">
         <v>16</v>
       </c>
       <c r="F30" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="G30" t="s" s="2">
         <v>35</v>
-      </c>
-      <c r="G30" t="s" s="2">
-        <v>36</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -2076,7 +2073,7 @@
         <v>80</v>
       </c>
       <c r="D31" t="s" s="2">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s" s="2">
         <v>16</v>
@@ -2101,7 +2098,7 @@
         <v>1800</v>
       </c>
       <c r="D32" t="s" s="2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E32" t="s" s="2">
         <v>7</v>
@@ -2126,7 +2123,7 @@
         <v>800</v>
       </c>
       <c r="D33" t="s" s="2">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s" s="2">
         <v>13</v>
@@ -2151,7 +2148,7 @@
         <v>75.5</v>
       </c>
       <c r="D34" t="s" s="2">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s" s="2">
         <v>16</v>

</xml_diff>